<commit_message>
css update & js refactor
</commit_message>
<xml_diff>
--- a/export/Gymnázium a ZUŠ Šlapanice.xlsx
+++ b/export/Gymnázium a ZUŠ Šlapanice.xlsx
@@ -671,7 +671,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>Pavelka</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -681,7 +681,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>asd</t>
+          <t>V2C</t>
         </is>
       </c>
       <c r="H7" t="n">
@@ -695,13 +695,6 @@
       <c r="B8" t="n">
         <v>0</v>
       </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -710,13 +703,6 @@
       <c r="B9" t="n">
         <v>37</v>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -725,26 +711,12 @@
       <c r="B10" t="n">
         <v>0</v>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
         <v>86</v>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>